<commit_message>
Nav-komponentti. Gitignore Officesovellusten väliaikaistiedostoille.
</commit_message>
<xml_diff>
--- a/dokumentaatio/Devauspaivakirja.xlsx
+++ b/dokumentaatio/Devauspaivakirja.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YouSports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YouSports\dokumentaatio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361F6F1C-CF49-4C34-AE33-98FD1CB35AAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB22B50-E43F-44EB-B696-3E5AA381095F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A84D29A5-6838-4082-89A1-87CB0042D78E}"/>
+    <workbookView xWindow="5355" yWindow="5100" windowWidth="21600" windowHeight="11385" xr2:uid="{A84D29A5-6838-4082-89A1-87CB0042D78E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>pvm</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Use case suunnittelu</t>
+  </si>
+  <si>
+    <t>Nav komponentti</t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858A7ECA-FD19-4A73-9498-6038A34B7408}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,6 +522,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44271</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Testaa boxscoren haku fronttiin. Ylimääräisiä kommentteja ja loggauksia pois
</commit_message>
<xml_diff>
--- a/dokumentaatio/Devauspaivakirja.xlsx
+++ b/dokumentaatio/Devauspaivakirja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YouSports\dokumentaatio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC48132-C55C-4A28-B135-DD87B3FD79B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7012A66F-BE30-4C58-9181-E51931A68031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A84D29A5-6838-4082-89A1-87CB0042D78E}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{A84D29A5-6838-4082-89A1-87CB0042D78E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>pvm</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Nav komponentti responsiiviseksi</t>
+  </si>
+  <si>
+    <t>Mieleenpalautus :D Testaa boxscoren fetchaus</t>
   </si>
 </sst>
 </file>
@@ -447,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858A7ECA-FD19-4A73-9498-6038A34B7408}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +477,7 @@
       </c>
       <c r="I1" cm="1">
         <f t="array" ref="I1">SUM(B2:B999/60)</f>
-        <v>11.916666666666666</v>
+        <v>12.583333333333332</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -577,6 +580,17 @@
       </c>
       <c r="C10" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44460</v>
+      </c>
+      <c r="B11">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nba esimerkki omaan komponenttiin
</commit_message>
<xml_diff>
--- a/dokumentaatio/Devauspaivakirja.xlsx
+++ b/dokumentaatio/Devauspaivakirja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YouSports\dokumentaatio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7012A66F-BE30-4C58-9181-E51931A68031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5460760-CD8E-42DB-A819-94905726CF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{A84D29A5-6838-4082-89A1-87CB0042D78E}"/>
   </bookViews>
@@ -97,7 +97,7 @@
     <t>Nav komponentti responsiiviseksi</t>
   </si>
   <si>
-    <t>Mieleenpalautus :D Testaa boxscoren fetchaus</t>
+    <t>Mieleenpalautus :D Home ja Nba komponentteja</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +477,7 @@
       </c>
       <c r="I1" cm="1">
         <f t="array" ref="I1">SUM(B2:B999/60)</f>
-        <v>12.583333333333332</v>
+        <v>13.916666666666666</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -587,7 +587,7 @@
         <v>44460</v>
       </c>
       <c r="B11">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Aloitettu draw.io dokumentaatio: Frontend luokkadiagrammi
</commit_message>
<xml_diff>
--- a/dokumentaatio/Devauspaivakirja.xlsx
+++ b/dokumentaatio/Devauspaivakirja.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YouSports\dokumentaatio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C40AB8-132D-4BA5-98D9-4254D19DB69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A985F7A4-FDF5-45FD-9E00-00F1C6155D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A84D29A5-6838-4082-89A1-87CB0042D78E}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>pvm</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Reduxin käyttö ja päivämäärän kanssa nba scoreboardille</t>
+  </si>
+  <si>
+    <t>Debuggia päivämäärien ja scorejen kanssa</t>
+  </si>
+  <si>
+    <t>Päivämäärän hallinta toimii nyt, alotettu draw.io dokumentaatio</t>
   </si>
 </sst>
 </file>
@@ -139,10 +145,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,49 +466,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858A7ECA-FD19-4A73-9498-6038A34B7408}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" customWidth="1"/>
+    <col min="3" max="3" width="76.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" cm="1">
-        <f t="array" ref="I1">SUM(B2:B999/60)</f>
-        <v>18.916666666666664</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F1" cm="1">
+        <f t="array" ref="F1">SUM(B2:B999/60)</f>
+        <v>21.249999999999996</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44238</v>
       </c>
       <c r="B2">
         <v>60</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44239</v>
       </c>
@@ -507,44 +516,44 @@
         <f>45+50</f>
         <v>95</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44243</v>
       </c>
       <c r="B4">
         <v>50</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44245</v>
       </c>
       <c r="B5">
         <v>90</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44248</v>
       </c>
       <c r="B6">
         <v>150</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44249</v>
       </c>
@@ -552,11 +561,11 @@
         <f>10+70</f>
         <v>80</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44259</v>
       </c>
@@ -564,63 +573,85 @@
         <f>30</f>
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44271</v>
       </c>
       <c r="B9">
         <v>100</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44281</v>
       </c>
       <c r="B10">
         <v>60</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44460</v>
       </c>
       <c r="B11">
         <v>120</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44481</v>
       </c>
       <c r="B12" s="2">
         <v>180</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44482</v>
       </c>
       <c r="B13" s="2">
         <v>120</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44492</v>
+      </c>
+      <c r="B14" s="2">
+        <v>60</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44590</v>
+      </c>
+      <c r="B15" s="2">
+        <v>80</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lisätty tilastojen haku ja niiden näyttö Nba välilehdellä
</commit_message>
<xml_diff>
--- a/dokumentaatio/Devauspaivakirja.xlsx
+++ b/dokumentaatio/Devauspaivakirja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YouSports\dokumentaatio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A985F7A4-FDF5-45FD-9E00-00F1C6155D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A905FF00-A342-49C2-A160-898FCD19586E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A84D29A5-6838-4082-89A1-87CB0042D78E}"/>
   </bookViews>
@@ -109,7 +109,7 @@
     <t>Debuggia päivämäärien ja scorejen kanssa</t>
   </si>
   <si>
-    <t>Päivämäärän hallinta toimii nyt, alotettu draw.io dokumentaatio</t>
+    <t>Päivämäärän hallinta toimii nyt, alotettu draw.io dokumentaatio, statseja Nba komponenttiin</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +494,7 @@
       </c>
       <c r="F1" cm="1">
         <f t="array" ref="F1">SUM(B2:B999/60)</f>
-        <v>21.249999999999996</v>
+        <v>23.583333333333332</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -643,12 +643,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44590</v>
       </c>
       <c r="B15" s="2">
-        <v>80</v>
+        <f>80+34+16+30+60</f>
+        <v>220</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
DateSelector ja Scoreboard omiin komponentteihin. Conditional rendering sen mukaan, lataako tai onko pelejä päivällä.
</commit_message>
<xml_diff>
--- a/dokumentaatio/Devauspaivakirja.xlsx
+++ b/dokumentaatio/Devauspaivakirja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YouSports\dokumentaatio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A905FF00-A342-49C2-A160-898FCD19586E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4FE7E6-61F1-4CEF-9FBF-2E8DA6C746CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A84D29A5-6838-4082-89A1-87CB0042D78E}"/>
+    <workbookView xWindow="7275" yWindow="105" windowWidth="19200" windowHeight="15495" xr2:uid="{A84D29A5-6838-4082-89A1-87CB0042D78E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>pvm</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Päivämäärän hallinta toimii nyt, alotettu draw.io dokumentaatio, statseja Nba komponenttiin</t>
+  </si>
+  <si>
+    <t>Nba komponentin proton jatkamista loppuun</t>
   </si>
 </sst>
 </file>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858A7ECA-FD19-4A73-9498-6038A34B7408}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +497,7 @@
       </c>
       <c r="F1" cm="1">
         <f t="array" ref="F1">SUM(B2:B999/60)</f>
-        <v>23.583333333333332</v>
+        <v>26.583333333333332</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -653,6 +656,18 @@
       </c>
       <c r="C15" s="3" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44614</v>
+      </c>
+      <c r="B16" s="2">
+        <f>60+120</f>
+        <v>180</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modularisointi ja mongo alustus
</commit_message>
<xml_diff>
--- a/dokumentaatio/Devauspaivakirja.xlsx
+++ b/dokumentaatio/Devauspaivakirja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YouSports\dokumentaatio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0A4EED-EAEC-414F-9A36-942506FB7805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517B9373-3705-450E-993B-F74A39242F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1140" windowWidth="29040" windowHeight="15840" xr2:uid="{A84D29A5-6838-4082-89A1-87CB0042D78E}"/>
   </bookViews>
@@ -115,7 +115,7 @@
     <t>Nba komponentin proton jatkamista loppuun</t>
   </si>
   <si>
-    <t>init backend</t>
+    <t>init backend, modularisointi ja mongoose alustus</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +500,7 @@
       </c>
       <c r="F1" cm="1">
         <f t="array" ref="F1">SUM(B2:B999/60)</f>
-        <v>27.583333333333332</v>
+        <v>28.083333333333332</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -678,7 +678,8 @@
         <v>44626</v>
       </c>
       <c r="B17" s="2">
-        <v>60</v>
+        <f>50 + 40</f>
+        <v>90</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>19</v>

</xml_diff>